<commit_message>
Negative scenarios for bank manager workflow added
</commit_message>
<xml_diff>
--- a/TestingBankOperations/TestData/CustomerList.xlsx
+++ b/TestingBankOperations/TestData/CustomerList.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z0042JXJ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z0042JXJ\Desktop\Self-study\TestingBankOperations\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034B16DF-8E0C-4027-B41A-9A982DFC894B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE236C63-DA7A-4A19-9F89-E66231E155CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4E59F1C-6211-4434-B933-F4F4923A6DBE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4E59F1C-6211-4434-B933-F4F4923A6DBE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PostitiveEntries" sheetId="1" r:id="rId1"/>
+    <sheet name="NegativeEntries" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>${FNAME}</t>
   </si>
@@ -80,6 +81,21 @@
   </si>
   <si>
     <t>Bourne</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>Vishal</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Kapoor</t>
+  </si>
+  <si>
+    <t>${EMPTY}</t>
   </si>
 </sst>
 </file>
@@ -440,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9760ACA5-7416-4930-88B9-F872BC707CCD}">
   <dimension ref="B1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,4 +545,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A74E443-9BA2-48A3-8C3E-87B1DCD93153}">
+  <dimension ref="B1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>67890</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Customer login workflow implemented and tested
End to end workflow (Bank manager & Customer) implemented and tested
</commit_message>
<xml_diff>
--- a/TestingBankOperations/TestData/CustomerList.xlsx
+++ b/TestingBankOperations/TestData/CustomerList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z0042JXJ\Desktop\Self-study\TestingBankOperations\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE236C63-DA7A-4A19-9F89-E66231E155CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9607DB2-2635-43B5-B27D-FD276EB7BB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4E59F1C-6211-4434-B933-F4F4923A6DBE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4E59F1C-6211-4434-B933-F4F4923A6DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="PostitiveEntries" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>${FNAME}</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>${EMPTY}</t>
+  </si>
+  <si>
+    <t>${DEPOSIT}</t>
+  </si>
+  <si>
+    <t>${WITHDRAWL}</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9760ACA5-7416-4930-88B9-F872BC707CCD}">
-  <dimension ref="B1:I5"/>
+  <dimension ref="B1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,9 +471,11 @@
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +492,15 @@
         <v>3</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -498,8 +513,14 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -512,8 +533,14 @@
       <c r="H3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>1234</v>
+      </c>
+      <c r="L3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -526,8 +553,14 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>89500</v>
+      </c>
+      <c r="L4">
+        <v>84000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -539,6 +572,12 @@
       </c>
       <c r="H5" t="s">
         <v>6</v>
+      </c>
+      <c r="J5">
+        <v>1100</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -551,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A74E443-9BA2-48A3-8C3E-87B1DCD93153}">
   <dimension ref="B1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,6 +599,7 @@
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>